<commit_message>
CSG1132 A2: added wilcox rank sum test results, needs justificiation
</commit_message>
<xml_diff>
--- a/year_1/sem_1/CSG1132_communicating_in_an_it_environment/0c_assignment_2/dev/rstudio/fbDataset_FINAL.xlsx
+++ b/year_1/sem_1/CSG1132_communicating_in_an_it_environment/0c_assignment_2/dev/rstudio/fbDataset_FINAL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17475" windowHeight="12150" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17475" windowHeight="12150"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="59">
   <si>
     <t>Age</t>
   </si>
@@ -204,12 +204,6 @@
   </si>
   <si>
     <t>T TEST</t>
-  </si>
-  <si>
-    <t>2 TAIL</t>
-  </si>
-  <si>
-    <t>P-Value</t>
   </si>
 </sst>
 </file>
@@ -949,9 +943,6 @@
       <sheetName val="Ken Tau Table"/>
     </sheetNames>
     <definedNames>
-      <definedName name="MANN"/>
-      <definedName name="MPROB"/>
-      <definedName name="MTEST"/>
       <definedName name="RANK_SUM"/>
       <definedName name="SRankCRIT"/>
       <definedName name="SRankPair"/>
@@ -1235,10 +1226,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="L1:AA17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,7 +1761,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>19</v>
       </c>
@@ -1801,7 +1793,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1832,29 +1824,8 @@
       <c r="J18">
         <v>15</v>
       </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="W18" t="s">
-        <v>29</v>
-      </c>
-      <c r="X18" s="13" t="str">
-        <f>IF('FB FRIENDS'!AB17&lt;'FB FRIENDS'!AB10,"yes","no")</f>
-        <v>yes</v>
-      </c>
-      <c r="Y18" s="14" t="str">
-        <f>IF('FB FRIENDS'!AC17&lt;'FB FRIENDS'!AB10,"yes","no")</f>
-        <v>yes</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1886,7 +1857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1918,7 +1889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1950,7 +1921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -1982,7 +1953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18</v>
       </c>
@@ -2014,7 +1985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>17</v>
       </c>
@@ -2046,7 +2017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>18</v>
       </c>
@@ -2078,7 +2049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>19</v>
       </c>
@@ -2110,7 +2081,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>18</v>
       </c>
@@ -2141,17 +2112,8 @@
       <c r="J27">
         <v>7</v>
       </c>
-      <c r="AB27" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC27" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>21</v>
       </c>
@@ -2182,20 +2144,8 @@
       <c r="J28">
         <v>4</v>
       </c>
-      <c r="AB28">
-        <f>[1]!MTEST(B2:B49,E2:E49,2)</f>
-        <v>3.1347998294848486E-17</v>
-      </c>
-      <c r="AC28">
-        <f>[1]!MANN(B2:B49,E2:E49)</f>
-        <v>0</v>
-      </c>
-      <c r="AD28" t="e">
-        <f>[1]!MPROB(0,48,48,2,40)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>19</v>
       </c>
@@ -2227,7 +2177,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>24</v>
       </c>
@@ -2259,7 +2209,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>17</v>
       </c>
@@ -2291,7 +2241,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>23</v>
       </c>
@@ -2877,7 +2827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>

</xml_diff>